<commit_message>
modified the rest of the input files for taf trait import
</commit_message>
<xml_diff>
--- a/src/files/TraitImport_v03/test_import-xlsx.xlsx
+++ b/src/files/TraitImport_v03/test_import-xlsx.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daw279\Documents\Testing\Cucumber\BI_Cucumber\BI_Gherkin_Scenarios_v02\Trait Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daw279\taf\src\files\TraitImport_v03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25427" windowHeight="12660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25428" windowHeight="12660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
   <si>
     <t>Column</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>Package</t>
+  </si>
+  <si>
+    <t>Tags</t>
   </si>
 </sst>
 </file>
@@ -900,10 +903,10 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.05859375" customWidth="1"/>
-    <col min="2" max="2" width="155.17578125" customWidth="1"/>
+    <col min="1" max="1" width="19.0546875" customWidth="1"/>
+    <col min="2" max="2" width="155.1640625" customWidth="1"/>
     <col min="3" max="3" width="74" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1126,15 +1129,15 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.17578125" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>52</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
[BI-1068] changed some READMEs and fixed maxmin file
</commit_message>
<xml_diff>
--- a/src/files/TraitImport_v03/test_import-xlsx.xlsx
+++ b/src/files/TraitImport_v03/test_import-xlsx.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25428" windowHeight="12660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25428" windowHeight="12660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="94">
   <si>
     <t>Column</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>active</t>
-  </si>
-  <si>
-    <t>Trait lists</t>
   </si>
   <si>
     <t>Favorites lists the trait should be added to, if any. Separate values with ;</t>
@@ -899,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -989,87 +986,87 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
       </c>
       <c r="C15" s="5">
         <v>2</v>
@@ -1077,10 +1074,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
       </c>
       <c r="C16" s="5">
         <v>2</v>
@@ -1088,10 +1085,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
       </c>
       <c r="C17" s="5">
         <v>9999</v>
@@ -1099,18 +1096,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -1139,7 +1136,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>6</v>
@@ -1148,178 +1145,178 @@
         <v>9</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="15" t="s">
-        <v>59</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
@@ -1327,37 +1324,37 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -1365,37 +1362,37 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" t="s">
-        <v>90</v>
-      </c>
       <c r="K7" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>

</xml_diff>

<commit_message>
trait import v0.4 changes
</commit_message>
<xml_diff>
--- a/src/files/TraitImport_v03/test_import-xlsx.xlsx
+++ b/src/files/TraitImport_v03/test_import-xlsx.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daw279\Documents\Testing\Cucumber\BI_Cucumber\BI_Gherkin_Scenarios_v02\Trait Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daw279\Documents\Testing\Cucumber\BI_Cucumber\TraitImportFiles\v0.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25427" windowHeight="12660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25428" windowHeight="12660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="Template" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="95">
   <si>
     <t>Column</t>
   </si>
@@ -85,9 +85,6 @@
     <t>active</t>
   </si>
   <si>
-    <t>Trait lists</t>
-  </si>
-  <si>
     <t>Favorites lists the trait should be added to, if any. Separate values with ;</t>
   </si>
   <si>
@@ -178,18 +175,9 @@
     <t>* Required field</t>
   </si>
   <si>
-    <t>Trait name</t>
-  </si>
-  <si>
     <t>Trait description</t>
   </si>
   <si>
-    <t>Trait level</t>
-  </si>
-  <si>
-    <t>Method name</t>
-  </si>
-  <si>
     <t>Method description</t>
   </si>
   <si>
@@ -302,13 +290,28 @@
   </si>
   <si>
     <t>Package</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Ontology term name</t>
+  </si>
+  <si>
+    <t>Trait entity</t>
+  </si>
+  <si>
+    <t>Trait attribute</t>
+  </si>
+  <si>
+    <t>damage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -320,23 +323,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,30 +339,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="26"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
+        <fgColor indexed="34"/>
         <bgColor indexed="13"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-        <bgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="46"/>
-        <bgColor indexed="24"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -386,44 +356,16 @@
       <left style="thin">
         <color indexed="63"/>
       </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -439,27 +381,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,13 +825,13 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.05859375" customWidth="1"/>
-    <col min="2" max="2" width="155.17578125" customWidth="1"/>
+    <col min="1" max="1" width="19.0546875" customWidth="1"/>
+    <col min="2" max="2" width="155.1640625" customWidth="1"/>
     <col min="3" max="3" width="74" customWidth="1"/>
   </cols>
   <sheetData>
@@ -986,87 +914,87 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
       </c>
       <c r="C15" s="5">
         <v>2</v>
@@ -1074,10 +1002,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
       </c>
       <c r="C16" s="5">
         <v>2</v>
@@ -1085,10 +1013,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
       </c>
       <c r="C17" s="5">
         <v>9999</v>
@@ -1096,18 +1024,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1126,277 +1054,278 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="F3" sqref="F3:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.17578125" customWidth="1"/>
+    <col min="1" max="1" width="30.609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.94140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="14.35" x14ac:dyDescent="0.5">
-      <c r="A1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="L1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>59</v>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>84</v>
+        <v>62</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K2" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="L2" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>85</v>
+        <v>63</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K3" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="L3" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>86</v>
+        <v>64</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="I4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="L4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" t="s">
-        <v>91</v>
-      </c>
-      <c r="K5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="L5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>82</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>88</v>
+        <v>66</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" t="s">
-        <v>83</v>
+        <v>89</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J6" t="s">
-        <v>90</v>
-      </c>
-      <c r="K6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>82</v>
-      </c>
+      <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" t="s">
-        <v>83</v>
+      <c r="F7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" t="s">
+        <v>79</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" t="s">
-        <v>90</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="L7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>82</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>